<commit_message>
Added Socket Data Filtering & Test
</commit_message>
<xml_diff>
--- a/demo.xlsx
+++ b/demo.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -451,64 +451,64 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>BINANCE_SPOT_MATIC_USDT</t>
+          <t>BINANCE_SPOT_ADA_USDT</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>36/1    ↘</t>
+          <t>0/0    ↘</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>8/1    ↗</t>
+          <t>0/0    ↘</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>7/0    ↗</t>
+          <t>0/0    ↘</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0/0    ↘</t>
+          <t>0/0    ↗</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>0/0    ↗</t>
+          <t>0/0    ↘</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>BINANCE_SPOT_LUNA_USDT</t>
+          <t>BINANCE_SPOT_BTC_USDT</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>0/0    ↘</t>
+          <t>1/0    ↘</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>12/2    ↗</t>
+          <t>5/1    ↘</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>9/2    ↘</t>
+          <t>6/1    ↘</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>0/0    ↘</t>
+          <t>1/0    ↗</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>7/2    ↘</t>
+          <t>0/0    ↘</t>
         </is>
       </c>
     </row>
@@ -520,17 +520,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>110/17    ↘</t>
+          <t>1/0    ↘</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1/0    ↘</t>
+          <t>0/0    ↘</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>8/1    ↘</t>
+          <t>5/1    ↘</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -540,7 +540,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>0/0    ↗</t>
+          <t>0/0    ↘</t>
         </is>
       </c>
     </row>
@@ -552,12 +552,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>12/2    ↘</t>
+          <t>0/0    ↘</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>8/0    ↗</t>
+          <t>0/0    ↘</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -567,12 +567,12 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1/0    ↘</t>
+          <t>0/0    ↗</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>0/0    ↗</t>
+          <t>0/0    ↘</t>
         </is>
       </c>
     </row>
@@ -584,22 +584,22 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>56/12    ↘</t>
+          <t>9/2    ↗</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>7/1    ↗</t>
+          <t>0/0    ↗</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0/0    ↘</t>
+          <t>0/0    ↗</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0/0    ↘</t>
+          <t>0/0    ↗</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -616,12 +616,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>71/14    ↘</t>
+          <t>0/0    ↘</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1/0    ↗</t>
+          <t>0/0    ↗</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -631,12 +631,12 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0/0    ↘</t>
+          <t>0/0    ↗</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>0/0    ↗</t>
+          <t>2/0    ↗</t>
         </is>
       </c>
     </row>
@@ -648,17 +648,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>119/49    ↘</t>
+          <t>1/0    ↘</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>4/1    ↘</t>
+          <t>5/1    ↘</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2/0    ↘</t>
+          <t>6/1    ↘</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -668,7 +668,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>0/0    ↗</t>
+          <t>0/0    ↘</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Merged socket & rest
</commit_message>
<xml_diff>
--- a/demo.xlsx
+++ b/demo.xlsx
@@ -451,7 +451,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>BINANCE_SPOT_ADA_USDT</t>
+          <t>BINANCE_SPOT_MATIC_USDT</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -461,17 +461,17 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0/0    ↘</t>
+          <t>0/0    ↗</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0/0    ↘</t>
+          <t>2/0    ↗</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0/0    ↗</t>
+          <t>0/0    ↘</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -483,32 +483,32 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>BINANCE_SPOT_BTC_USDT</t>
+          <t>BINANCE_SPOT_LUNA_USDT</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>0/0    ↘</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>0/0    ↗</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>0/0    ↗</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>0/0    ↗</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
           <t>1/0    ↘</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>5/1    ↘</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>6/1    ↘</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>1/0    ↗</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>0/0    ↘</t>
         </is>
       </c>
     </row>
@@ -520,22 +520,22 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1/0    ↘</t>
+          <t>0/0    ↗</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0/0    ↘</t>
+          <t>0/0    ↗</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>5/1    ↘</t>
+          <t>2/0    ↘</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0/0    ↘</t>
+          <t>2/0    ↘</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -552,12 +552,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>0/0    ↘</t>
+          <t>2/0    ↗</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0/0    ↘</t>
+          <t>0/0    ↗</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -567,12 +567,12 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0/0    ↗</t>
+          <t>0/0    ↘</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>0/0    ↘</t>
+          <t>1/0    ↘</t>
         </is>
       </c>
     </row>
@@ -584,7 +584,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>9/2    ↗</t>
+          <t>1/0    ↘</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -594,17 +594,17 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0/0    ↗</t>
+          <t>0/0    ↘</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0/0    ↗</t>
+          <t>0/0    ↘</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>0/0    ↗</t>
+          <t>0/0    ↘</t>
         </is>
       </c>
     </row>
@@ -631,12 +631,12 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0/0    ↗</t>
+          <t>1/0    ↘</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2/0    ↗</t>
+          <t>1/0    ↘</t>
         </is>
       </c>
     </row>
@@ -648,27 +648,27 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
+          <t>4/1    ↘</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>0/0    ↗</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>0/0    ↘</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
           <t>1/0    ↘</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>5/1    ↘</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>6/1    ↘</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>1/0    ↗</t>
-        </is>
-      </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>0/0    ↘</t>
+          <t>1/0    ↘</t>
         </is>
       </c>
     </row>

</xml_diff>